<commit_message>
Edited Objective 1 codes
</commit_message>
<xml_diff>
--- a/Data sets/200204_philippines-2019-events-data.xlsx_3FAWSAccessKeyId=AKIAXYC32WNARK756OUG_Expires=1644193427_Signature=hFTPcWroN6S3M2pX40ObWvu24p8=.xlsx
+++ b/Data sets/200204_philippines-2019-events-data.xlsx_3FAWSAccessKeyId=AKIAXYC32WNARK756OUG_Expires=1644193427_Signature=hFTPcWroN6S3M2pX40ObWvu24p8=.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surge\Desktop\ITBA-3207_TeamTyphoonAnalysts\Data sets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johna\Desktop\ITBA-3207_TeamTyphoonAnalysts\Data sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC4CB17-9CAC-4C43-8A0F-CF17B71DB1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F115F38C-B614-4512-BD03-B2B90451F67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5027,8 +5027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>